<commit_message>
before merge road, git it.
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
         <v>101.87</v>
       </c>
       <c r="D2">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -558,7 +558,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
completed merge load drawing, now change input vechile algothimn
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G40" sqref="A3:G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,16 +527,16 @@
         <v>101.87</v>
       </c>
       <c r="D2">
-        <v>65000</v>
+        <v>200000</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
completed function about back car to the start place.
[todo]
1. check change lances and update velocity.
2. modify bug: two car will be too close sometimes.
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="925" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="parsed mile posts" sheetId="1" state="visible" r:id="rId2"/>
@@ -239,7 +239,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -285,25 +285,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>100.93</v>
+        <v>9.96</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>101.87</v>
+        <v>10.56</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>65000</v>
+        <v>147000</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>100.93</v>

</xml_diff>

<commit_message>
refactoring: delete function iterator; modify: the axis of subplot, make all of subplot has the same x-axis and y-axis. [todo]: 1. check: if the relation between density and volume is normal. 2. repair bug: to_next_path function run abnormally 3. check: if change lanes run normally. 4. check: if update velocity run normally. 5. repair bug: two car will be too close sometimes.
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Route_ID</t>
   </si>
@@ -236,10 +236,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -302,8 +302,28 @@
       <c r="G2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>100.93</v>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10.56</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>10.93</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>177000</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -325,7 +345,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="A4:J5 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
repair bugs of change lanes and update velocity has found 1. find_nearest_car will ignore the car which in the same place and different lane 2. write around_cars['r-'] to around_cars['r+'] by mistake. 3. forward_cars should be calculated after execute "change_lanes" function
[todo]:
1. check: if the relation between density and volume is normal.
2. repair bug: to_next_path function run abnormally
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Route_ID</t>
   </si>
@@ -236,10 +236,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:J5"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -285,7 +285,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>9.96</v>
+        <v>10.15</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>10.56</v>
@@ -300,30 +300,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>10.56</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>10.93</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>177000</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -345,7 +322,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="A4:J5 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
adjust the ideal volume and and the real volume:     1. initial cars will created with random place     2. if can not find a suit place in to_next_path, we will initialize another new car with new car id and the same location.
    [todo]:
    1. repair bug: function should consider the situation of next milepost path when "output" from this milepost path
    2. check: if the relation between density and volume is normal.
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -238,8 +238,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -288,10 +288,10 @@
         <v>10.15</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>10.56</v>
+        <v>11.56</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>147000</v>
+        <v>50000</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -300,7 +300,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -321,7 +321,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
repair bug: function should consider the situation of next milepost path when "output" from this milepost path     1. add function update_next_path_info to contact the information between two path, include path_map and car_dictory.     2. modify the logic of Handler.update, we should do path.update, then do path.add_car     3. modify the logic of Path.find_nearest_car, the nearest car come from car_dictory and next_car_dictory, the place of car in next_car_dict
    [todo]:
    1. check: if the relation between density and volume is normal.
    2. check: if the function of change lanes run normally.
    3. repair bug: add car to next path will be failed sometimes when use v_forward_imaginary
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Route_ID</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>IS</t>
+  </si>
+  <si>
+    <t>Intersection with I90</t>
   </si>
   <si>
     <t>Definitions</t>
@@ -236,10 +239,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -302,6 +305,56 @@
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10.15</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10.15</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -334,7 +387,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,58 +395,58 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the relation of density, volume and velocity in our program is normal now. 1. use poly to fitting the relation of above three, the result is perfect! change lanes function run normally. 1. after change lanes, car will has new car id. 2. use 'x' label to mark 'change lanes' car.
[todo]:
1. check: if the function merge lanes in serveral milepost run normally.
2. repair bug: add car to next path will be failed sometimes when use v_forward_imaginary
3. add auto_car behavior
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Route_ID</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>IS</t>
-  </si>
-  <si>
-    <t>Intersection with I90</t>
   </si>
   <si>
     <t>Definitions</t>
@@ -239,10 +236,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -294,7 +291,7 @@
         <v>11.56</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>50000</v>
+        <v>120000</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -305,56 +302,6 @@
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>10.15</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>11.56</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>10.15</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>11.56</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -387,7 +334,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,58 +342,58 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the function merge lanes in serveral milepost can run normally. 1. repair bug: I forget write last_cell_amount = cell_amount + last_cell_amount, make the label of change lanes appear in wrong place. 2. repair bug: I forget clear last_path after finish a iteration in driver function.     - the condition of execute last_path.update_next_path_info(path) is index != 0 not last_path!=0
[todo]
1. repair bug: add car to next path will be failed sometimes when use v_forward_imaginary
2. add auto_car behavior
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data2.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Route_ID</t>
   </si>
@@ -236,10 +236,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -301,6 +301,75 @@
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10.15</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>13.42</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>13.78</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>141000</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10.15</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>